<commit_message>
se soluciono el problema de Do Not Mark Days
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -73,7 +73,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill/>
     </fill>
@@ -338,6 +338,12 @@
         <bgColor rgb="00FFFF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -452,7 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -773,6 +779,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,10 +1258,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AWU14"/>
+  <dimension ref="A1:AWU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -56006,256 +56013,72 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Fuel Attendants</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Aloekoe Figaro</t>
+          <t>Rosa Merlano</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TP0904</t>
-        </is>
-      </c>
-      <c r="ARS12" s="108" t="inlineStr">
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="ARV12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ART12" s="108" t="inlineStr">
+      <c r="ARW12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARU12" s="108" t="inlineStr">
+      <c r="ARX12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARV12" s="108" t="inlineStr">
+      <c r="ARY12" s="108" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ARW12" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARX12" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARY12" s="109" t="inlineStr">
+      <c r="ARZ12" s="109" t="inlineStr">
         <is>
           <t>ON NS</t>
         </is>
       </c>
-      <c r="ARZ12" s="109" t="inlineStr">
+      <c r="ASA12" s="109" t="inlineStr">
         <is>
           <t>ON NS</t>
         </is>
       </c>
-      <c r="ASA12" s="109" t="inlineStr">
+      <c r="ASB12" s="109" t="inlineStr">
         <is>
           <t>ON NS</t>
         </is>
       </c>
-      <c r="ASB12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASC12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASD12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASE12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASF12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASG12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASH12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASI12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASJ12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Fuel Attendants</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Juan Hernandez</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>TP1234</t>
-        </is>
-      </c>
-      <c r="ARP13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARQ13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARR13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARS13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ART13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARU13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARV13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ARW13" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Rosa Merlano</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>TP0903</t>
-        </is>
-      </c>
-      <c r="ARP14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARQ14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARR14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARS14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ART14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARU14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARV14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARW14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARX14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARY14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ARZ14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASA14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASB14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASC14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASD14" s="108" t="inlineStr">
-        <is>
-          <t>ON</t>
+      <c r="ASD12" s="110" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="ASE12" s="110" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="ASF12" s="110" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="ASG12" s="110" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega el indicador de usuario logueado en la main_dinwos
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Operations_best_opt" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Operations_best_opt" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:AWU12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -56018,7 +56018,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rosa Merlano</t>
+          <t>Rosa Melano</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -56046,39 +56046,24 @@
           <t>ON</t>
         </is>
       </c>
-      <c r="ARZ12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASA12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASB12" s="109" t="inlineStr">
-        <is>
-          <t>ON NS</t>
-        </is>
-      </c>
-      <c r="ASD12" s="110" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="ASE12" s="110" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="ASF12" s="110" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="ASG12" s="110" t="inlineStr">
-        <is>
-          <t>OFF</t>
+      <c r="ARZ12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASA12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASB12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASC12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega el audit log
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Operations_best_opt" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Operations_best_opt" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -56066,6 +56066,21 @@
           <t>ON</t>
         </is>
       </c>
+      <c r="ASG12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASH12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASI12" s="108" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
location funtional e interfaz grafica con el boton estable
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -52273,12 +52273,41 @@
         </is>
       </c>
       <c r="ASX9" s="106" t="n"/>
-      <c r="ASY9" s="106" t="n"/>
-      <c r="ASZ9" s="106" t="n"/>
-      <c r="ATA9" s="106" t="n"/>
-      <c r="ATB9" s="106" t="n"/>
-      <c r="ATC9" s="106" t="n"/>
-      <c r="ATD9" s="106" t="n"/>
+      <c r="ASY9" s="110" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASZ9" s="110" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATA9" s="110" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATB9" s="110" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATC9" s="110" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATD9" s="110" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATE9" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="30" customFormat="1" customHeight="1" s="8">
       <c r="A10" s="77" t="inlineStr">

</xml_diff>

<commit_message>
se agrega sincronizacion de BD to Excel, es decir informacion que no esta en el excel pero esta en la base de dato se reporta en el excel
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -73,7 +73,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="46">
     <fill>
       <patternFill/>
     </fill>
@@ -332,6 +332,18 @@
         <bgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF99"/>
+        <bgColor rgb="00FFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -446,7 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -772,6 +784,8 @@
     <xf numFmtId="46" fontId="5" fillId="43" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,6 +868,7 @@
   <authors>
     <author>None</author>
     <author>Data Analyst</author>
+    <author>ShiftType</author>
   </authors>
   <commentList>
     <comment ref="RY4" authorId="0" shapeId="0">
@@ -943,6 +958,31 @@
       <text>
         <t>Data Analyst:
 will take in July as compensation leave</t>
+      </text>
+    </comment>
+    <comment ref="ASN14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASO14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASP14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASQ14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASR14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
       </text>
     </comment>
   </commentList>
@@ -1250,7 +1290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AWU11"/>
+  <dimension ref="A1:AWU14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -56066,6 +56106,147 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Elver Gonzales</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TBT</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Site Manager</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Miguel Venegas</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GM123</t>
+        </is>
+      </c>
+      <c r="ARW13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARX13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARY13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARZ13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASA13" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASB13" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASC13" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Technician</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Rosa Melano</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MK1456</t>
+        </is>
+      </c>
+      <c r="ARY14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARZ14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASA14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASJ14" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASK14" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASL14" s="111" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASN14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASO14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASP14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASQ14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASR14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="YT7:YX7"/>

</xml_diff>

<commit_message>
se hace correcion de shift types en el preview
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -73,7 +73,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill/>
     </fill>
@@ -344,6 +344,12 @@
         <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0013E7FF"/>
+        <bgColor rgb="0013E7FF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -458,7 +464,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -786,6 +792,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,6 +965,46 @@
       <text>
         <t>Data Analyst:
 will take in July as compensation leave</t>
+      </text>
+    </comment>
+    <comment ref="ASY12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASZ12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ATA12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ATB12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ATC12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ATD12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ATE12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ATF12" authorId="2" shapeId="0">
+      <text>
+        <t>10:00-14:00</t>
       </text>
     </comment>
     <comment ref="ASN14" authorId="2" shapeId="0">
@@ -56122,6 +56169,46 @@
           <t>TBT</t>
         </is>
       </c>
+      <c r="ASY12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ASZ12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ATA12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ATB12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ATC12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ATD12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ATE12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="ATF12" s="113" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -56174,6 +56261,41 @@
           <t>ON NS</t>
         </is>
       </c>
+      <c r="ASY13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASZ13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATA13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATB13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATC13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATD13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATE13" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -56244,6 +56366,41 @@
       <c r="ASR14" s="112" t="inlineStr">
         <is>
           <t>S</t>
+        </is>
+      </c>
+      <c r="ASY14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASZ14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATA14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATB14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATC14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATD14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATE14" s="109" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
merge realizado, falta agregar problema de salida de  cierre de software al hacer login
</commit_message>
<xml_diff>
--- a/PlanStaffRGM.xlsx
+++ b/PlanStaffRGM.xlsx
@@ -73,7 +73,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill/>
     </fill>
@@ -344,6 +344,12 @@
         <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -458,7 +464,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -786,6 +792,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,6 +990,46 @@
     <comment ref="ASR14" authorId="2" shapeId="0">
       <text>
         <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASU14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASV14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASW14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ASX14" authorId="2" shapeId="0">
+      <text>
+        <t>08:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ATB14" authorId="2" shapeId="0">
+      <text>
+        <t>13:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ATC14" authorId="2" shapeId="0">
+      <text>
+        <t>13:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ATD14" authorId="2" shapeId="0">
+      <text>
+        <t>13:00-17:00</t>
+      </text>
+    </comment>
+    <comment ref="ATE14" authorId="2" shapeId="0">
+      <text>
+        <t>13:00-17:00</t>
       </text>
     </comment>
   </commentList>
@@ -56246,6 +56293,46 @@
           <t>S</t>
         </is>
       </c>
+      <c r="ASU14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASV14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASW14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ASX14" s="112" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="ATB14" s="113" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="ATC14" s="113" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="ATD14" s="113" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="ATE14" s="113" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>